<commit_message>
updated building energy use
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
+++ b/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
@@ -426,6 +426,74 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -26892,12 +26960,6 @@
           <t>Table HC2.1  Structural and geographic characteristics of U.S. homes by housing unit type, 20151</t>
         </is>
       </c>
-      <c r="B2" s="55" t="n"/>
-      <c r="C2" s="55" t="n"/>
-      <c r="D2" s="55" t="n"/>
-      <c r="E2" s="55" t="n"/>
-      <c r="F2" s="55" t="n"/>
-      <c r="G2" s="55" t="n"/>
     </row>
     <row r="3" ht="24" customHeight="1" s="52">
       <c r="A3" s="31" t="n"/>

</xml_diff>